<commit_message>
added the results of Seq2seq to dashboard
</commit_message>
<xml_diff>
--- a/Results/Dashboard.xlsx
+++ b/Results/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saad.LAKES\Desktop\Pavement-Temperature-Prediction\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AD658E-F1EE-41D6-8F8C-C552CD4765F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA9C20E-4790-41D8-BBF2-28C531ADFD43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{63DD03F2-C25F-4FEC-9FD3-D8FFAFAFBABA}"/>
   </bookViews>
@@ -21,9 +21,9 @@
     <definedName name="Slicer_Attention">#N/A</definedName>
     <definedName name="Slicer_Hours_Ahead">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="20">
   <si>
     <t>Attention</t>
   </si>
@@ -110,6 +110,9 @@
   <si>
     <t>With Attention</t>
   </si>
+  <si>
+    <t>Seq2Seq</t>
+  </si>
 </sst>
 </file>
 
@@ -162,35 +165,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -352,6 +326,35 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -913,41 +916,47 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pivots!$A$5:$A$9</c:f>
+              <c:f>Pivots!$A$5:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>ConvLSTM</c:v>
+                  <c:v>Seq2Seq</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>LSTM</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CNN-LSTM</c:v>
+                  <c:v>ConvLSTM</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Wavenet</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CNN-LSTM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pivots!$B$5:$B$9</c:f>
+              <c:f>Pivots!$B$5:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.3517157260161525</c:v>
+                  <c:v>5.0079818549785262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4873572839496347</c:v>
+                  <c:v>6.0101463709468685</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4789816481064939</c:v>
+                  <c:v>6.1514877080625645</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2839149973115331</c:v>
+                  <c:v>6.5426767587242587</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6814087049809165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1043,41 +1052,47 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pivots!$A$5:$A$9</c:f>
+              <c:f>Pivots!$A$5:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>ConvLSTM</c:v>
+                  <c:v>Seq2Seq</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>LSTM</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CNN-LSTM</c:v>
+                  <c:v>ConvLSTM</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Wavenet</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CNN-LSTM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pivots!$C$5:$C$9</c:f>
+              <c:f>Pivots!$C$5:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.5096669559899261</c:v>
+                  <c:v>6.391382442590773</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3866020159812451</c:v>
+                  <c:v>6.3246772022361402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6113596632172205</c:v>
+                  <c:v>6.6903807124690626</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8843420402353912</c:v>
+                  <c:v>8.9135589438957474</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3131987559032101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1140,7 +1155,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.49497256768137621"/>
-              <c:y val="0.84136486528987575"/>
+              <c:y val="0.86147980326730855"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2030,8 +2045,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Hours Ahead">
@@ -2054,7 +2069,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2108,8 +2123,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>94951</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Attention">
@@ -2132,7 +2147,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2177,17 +2192,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="saad" refreshedDate="44154.56108900463" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="48" xr:uid="{615D4E70-7A9E-45F9-8419-B7C4B78E1522}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="saad" refreshedDate="44158.387588541664" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{615D4E70-7A9E-45F9-8419-B7C4B78E1522}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Model" numFmtId="0">
-      <sharedItems count="4">
+      <sharedItems count="5">
         <s v="Wavenet"/>
         <s v="LSTM"/>
         <s v="ConvLSTM"/>
         <s v="CNN-LSTM"/>
+        <s v="Seq2Seq"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Attention" numFmtId="0">
@@ -2236,7 +2252,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="48">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -2765,26 +2781,162 @@
     <n v="3.83"/>
     <x v="5"/>
   </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="0.99472862560344066"/>
+    <n v="1.8824611364964889"/>
+    <n v="1.3720281106801306"/>
+    <n v="0.96731107234679259"/>
+    <n v="3.8683369862557479E-2"/>
+    <n v="8.11"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1.0370251429241286"/>
+    <n v="1.9864738502694181"/>
+    <n v="1.4094232331948477"/>
+    <n v="0.96570426947297561"/>
+    <n v="4.1951367127826412E-2"/>
+    <n v="8.11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1.1340809811949129"/>
+    <n v="2.3479807320967274"/>
+    <n v="1.5323122175642689"/>
+    <n v="0.95966173693902013"/>
+    <n v="5.3778835137777731E-2"/>
+    <n v="8.11"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1.2301960530384493"/>
+    <n v="2.6251146570680395"/>
+    <n v="1.6202205581549813"/>
+    <n v="0.9550769087259009"/>
+    <n v="6.4024762796925372E-2"/>
+    <n v="8.11"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1.4225931963387886"/>
+    <n v="3.4471918109019404"/>
+    <n v="1.8566614691165271"/>
+    <n v="0.94117008621380893"/>
+    <n v="9.6459134625850526E-2"/>
+    <n v="8.11"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1.7159190986954318"/>
+    <n v="5.0079818549785262"/>
+    <n v="2.2378520628000693"/>
+    <n v="0.91465690797164778"/>
+    <n v="0.16871352804727779"/>
+    <n v="8.11"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1.1501555969109576"/>
+    <n v="2.4021636356663545"/>
+    <n v="1.5498914915781539"/>
+    <n v="0.95828644120451423"/>
+    <n v="5.6314286488135371E-2"/>
+    <n v="8.16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1.1856605795717334"/>
+    <n v="2.4969501103392542"/>
+    <n v="1.580174075961017"/>
+    <n v="0.95689108713311044"/>
+    <n v="5.961606258479242E-2"/>
+    <n v="8.16"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1.2295375897128085"/>
+    <n v="2.6426180084518007"/>
+    <n v="1.6256131177041482"/>
+    <n v="0.95459987429308257"/>
+    <n v="6.4812100514462026E-2"/>
+    <n v="8.16"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1.3715866256869456"/>
+    <n v="3.2522699297262427"/>
+    <n v="1.8034050930742773"/>
+    <n v="0.9443445190069224"/>
+    <n v="8.8352845628347013E-2"/>
+    <n v="8.16"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1.6222777218094457"/>
+    <n v="4.5054159599119767"/>
+    <n v="2.1225965136860037"/>
+    <n v="0.92311039041857057"/>
+    <n v="0.14397095894939954"/>
+    <n v="8.16"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1.9314381567356311"/>
+    <n v="6.391382442590773"/>
+    <n v="2.5281183600833987"/>
+    <n v="0.89108180584876384"/>
+    <n v="0.24286342126365276"/>
+    <n v="8.16"/>
+    <x v="5"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A33F6770-4ABB-4F87-976D-B13C6AD3E3D8}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A33F6770-4ABB-4F87-976D-B13C6AD3E3D8}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A3:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="5">
+      <items count="6">
         <item x="3"/>
         <item x="2"/>
         <item x="1"/>
         <item x="0"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
       <autoSortScope>
         <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
+          <references count="2">
             <reference field="4294967294" count="1" selected="0">
               <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="2"/>
             </reference>
           </references>
         </pivotArea>
@@ -2807,11 +2959,11 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
         <item x="5"/>
         <item t="default"/>
       </items>
@@ -2820,18 +2972,21 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="6">
     <i>
-      <x v="1"/>
+      <x v="4"/>
     </i>
     <i>
       <x v="2"/>
     </i>
     <i>
-      <x/>
+      <x v="1"/>
     </i>
     <i>
       <x v="3"/>
+    </i>
+    <i>
+      <x/>
     </i>
     <i t="grand">
       <x/>
@@ -2948,11 +3103,11 @@
   <data>
     <tabular pivotCacheId="1413685035">
       <items count="6">
-        <i x="0" s="1"/>
-        <i x="1" s="1"/>
-        <i x="2" s="1"/>
-        <i x="3" s="1"/>
-        <i x="4" s="1"/>
+        <i x="0"/>
+        <i x="1"/>
+        <i x="2"/>
+        <i x="3"/>
+        <i x="4"/>
         <i x="5" s="1"/>
       </items>
     </tabular>
@@ -2991,18 +3146,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A40C5364-D532-4850-BD71-B2C37FA582EC}" name="Table1" displayName="Table1" ref="A1:I49" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:I49" xr:uid="{ED0D47FB-18B8-4C67-9670-3E2CBE517802}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A40C5364-D532-4850-BD71-B2C37FA582EC}" name="Table1" displayName="Table1" ref="A1:I61" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:I61" xr:uid="{ED0D47FB-18B8-4C67-9670-3E2CBE517802}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{CF545063-03CF-401E-930A-816F89247E2E}" name="Model"/>
-    <tableColumn id="2" xr3:uid="{D95F79F9-E1DE-4634-A376-76E193012D40}" name="Attention" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{FB734E54-1D25-4C2D-AD8B-39527EEDAABA}" name="MAE" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{60154C47-3BE3-4E5B-A931-1E999CC0C5FE}" name="MSE" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{9E5FEA15-4FB9-43EA-B2D3-21FF74A30FAA}" name="RMSE" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{8F099E94-3629-4105-8223-CA7DDF8D9C37}" name="R2" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{D27EA600-3E43-4725-ABC3-B81E508957A2}" name="AGG" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{1D05D863-E2CE-4563-BB89-51FB596E89D4}" name="Time Taken" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{DC3A857A-91A6-4BE6-8A96-AB493AD8E254}" name="Hours Ahead" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D95F79F9-E1DE-4634-A376-76E193012D40}" name="Attention" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{FB734E54-1D25-4C2D-AD8B-39527EEDAABA}" name="MAE" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{60154C47-3BE3-4E5B-A931-1E999CC0C5FE}" name="MSE" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9E5FEA15-4FB9-43EA-B2D3-21FF74A30FAA}" name="RMSE" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{8F099E94-3629-4105-8223-CA7DDF8D9C37}" name="R2" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{D27EA600-3E43-4725-ABC3-B81E508957A2}" name="AGG" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{1D05D863-E2CE-4563-BB89-51FB596E89D4}" name="Time Taken" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{DC3A857A-91A6-4BE6-8A96-AB493AD8E254}" name="Hours Ahead" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3305,10 +3460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712E3C15-63C6-4140-A373-FF15B2D88EC3}">
-  <dimension ref="A3:D9"/>
+  <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3343,16 +3498,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4">
-        <v>3.3517157260161525</v>
+        <v>5.0079818549785262</v>
       </c>
       <c r="C5" s="4">
-        <v>3.5096669559899261</v>
+        <v>6.391382442590773</v>
       </c>
       <c r="D5" s="4">
-        <v>3.4306913410030391</v>
+        <v>5.6996821487846496</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3360,27 +3515,27 @@
         <v>10</v>
       </c>
       <c r="B6" s="4">
-        <v>3.4873572839496347</v>
+        <v>6.0101463709468685</v>
       </c>
       <c r="C6" s="4">
-        <v>3.3866020159812451</v>
+        <v>6.3246772022361402</v>
       </c>
       <c r="D6" s="4">
-        <v>3.4369796499654393</v>
+        <v>6.1674117865915044</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="4">
-        <v>4.4789816481064939</v>
+        <v>6.1514877080625645</v>
       </c>
       <c r="C7" s="4">
-        <v>3.6113596632172205</v>
+        <v>6.6903807124690626</v>
       </c>
       <c r="D7" s="4">
-        <v>4.045170655661857</v>
+        <v>6.4209342102658136</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3388,27 +3543,41 @@
         <v>9</v>
       </c>
       <c r="B8" s="4">
-        <v>4.2839149973115331</v>
+        <v>6.5426767587242587</v>
       </c>
       <c r="C8" s="4">
-        <v>5.8843420402353912</v>
+        <v>8.9135589438957474</v>
       </c>
       <c r="D8" s="4">
-        <v>5.0841285187734622</v>
+        <v>7.7281178513100031</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <v>7.6814087049809165</v>
+      </c>
+      <c r="C9" s="4">
+        <v>6.3131987559032101</v>
+      </c>
+      <c r="D9" s="4">
+        <v>6.9973037304420629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4">
-        <v>3.9004924138459534</v>
-      </c>
-      <c r="C9" s="4">
-        <v>4.0979926688559463</v>
-      </c>
-      <c r="D9" s="4">
-        <v>3.99924254135095</v>
+      <c r="B10" s="4">
+        <v>6.2787402795386269</v>
+      </c>
+      <c r="C10" s="4">
+        <v>6.9266396114189863</v>
+      </c>
+      <c r="D10" s="4">
+        <v>6.6026899454788062</v>
       </c>
     </row>
   </sheetData>
@@ -3421,7 +3590,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="X21" sqref="X21"/>
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3440,10 +3609,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380DC729-2475-4475-80B1-F9475DF84150}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4874,6 +5043,354 @@
         <v>6</v>
       </c>
     </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.99472862560344066</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1.8824611364964889</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1.3720281106801306</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0.96731107234679259</v>
+      </c>
+      <c r="G50" s="1">
+        <v>3.8683369862557479E-2</v>
+      </c>
+      <c r="H50" s="1">
+        <v>8.11</v>
+      </c>
+      <c r="I50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1.0370251429241286</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1.9864738502694181</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1.4094232331948477</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0.96570426947297561</v>
+      </c>
+      <c r="G51" s="1">
+        <v>4.1951367127826412E-2</v>
+      </c>
+      <c r="H51" s="1">
+        <v>8.11</v>
+      </c>
+      <c r="I51" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1.1340809811949129</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2.3479807320967274</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1.5323122175642689</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0.95966173693902013</v>
+      </c>
+      <c r="G52" s="1">
+        <v>5.3778835137777731E-2</v>
+      </c>
+      <c r="H52" s="1">
+        <v>8.11</v>
+      </c>
+      <c r="I52" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1.2301960530384493</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2.6251146570680395</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1.6202205581549813</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0.9550769087259009</v>
+      </c>
+      <c r="G53" s="1">
+        <v>6.4024762796925372E-2</v>
+      </c>
+      <c r="H53" s="1">
+        <v>8.11</v>
+      </c>
+      <c r="I53" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1.4225931963387886</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3.4471918109019404</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1.8566614691165271</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0.94117008621380893</v>
+      </c>
+      <c r="G54" s="1">
+        <v>9.6459134625850526E-2</v>
+      </c>
+      <c r="H54" s="1">
+        <v>8.11</v>
+      </c>
+      <c r="I54" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1.7159190986954318</v>
+      </c>
+      <c r="D55" s="1">
+        <v>5.0079818549785262</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2.2378520628000693</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0.91465690797164778</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0.16871352804727779</v>
+      </c>
+      <c r="H55" s="1">
+        <v>8.11</v>
+      </c>
+      <c r="I55" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1.1501555969109576</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2.4021636356663545</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1.5498914915781539</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0.95828644120451423</v>
+      </c>
+      <c r="G56" s="1">
+        <v>5.6314286488135371E-2</v>
+      </c>
+      <c r="H56" s="1">
+        <v>8.16</v>
+      </c>
+      <c r="I56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1.1856605795717334</v>
+      </c>
+      <c r="D57" s="1">
+        <v>2.4969501103392542</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1.580174075961017</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0.95689108713311044</v>
+      </c>
+      <c r="G57" s="1">
+        <v>5.961606258479242E-2</v>
+      </c>
+      <c r="H57" s="1">
+        <v>8.16</v>
+      </c>
+      <c r="I57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1.2295375897128085</v>
+      </c>
+      <c r="D58" s="1">
+        <v>2.6426180084518007</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1.6256131177041482</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0.95459987429308257</v>
+      </c>
+      <c r="G58" s="1">
+        <v>6.4812100514462026E-2</v>
+      </c>
+      <c r="H58" s="1">
+        <v>8.16</v>
+      </c>
+      <c r="I58" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1.3715866256869456</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3.2522699297262427</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1.8034050930742773</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0.9443445190069224</v>
+      </c>
+      <c r="G59" s="1">
+        <v>8.8352845628347013E-2</v>
+      </c>
+      <c r="H59" s="1">
+        <v>8.16</v>
+      </c>
+      <c r="I59" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1.6222777218094457</v>
+      </c>
+      <c r="D60" s="1">
+        <v>4.5054159599119767</v>
+      </c>
+      <c r="E60" s="1">
+        <v>2.1225965136860037</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0.92311039041857057</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0.14397095894939954</v>
+      </c>
+      <c r="H60" s="1">
+        <v>8.16</v>
+      </c>
+      <c r="I60" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1.9314381567356311</v>
+      </c>
+      <c r="D61" s="1">
+        <v>6.391382442590773</v>
+      </c>
+      <c r="E61" s="1">
+        <v>2.5281183600833987</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0.89108180584876384</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0.24286342126365276</v>
+      </c>
+      <c r="H61" s="1">
+        <v>8.16</v>
+      </c>
+      <c r="I61" s="1">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
conducted a test run on attention lstm and created new notebook
The test run on the lstm is being created to carry out the test and also a new notebook is created to do the development and then move code to the vs code
</commit_message>
<xml_diff>
--- a/Results/Dashboard.xlsx
+++ b/Results/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saad.LAKES\Desktop\Pavement-Temperature-Prediction\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA9C20E-4790-41D8-BBF2-28C531ADFD43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C437E593-7E77-470E-BE0D-CA4DC6AF6157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{63DD03F2-C25F-4FEC-9FD3-D8FFAFAFBABA}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -2917,7 +2917,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A33F6770-4ABB-4F87-976D-B13C6AD3E3D8}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A33F6770-4ABB-4F87-976D-B13C6AD3E3D8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">

</xml_diff>

<commit_message>
completed the wavenet run and also updated the dashboard
</commit_message>
<xml_diff>
--- a/Results/Dashboard.xlsx
+++ b/Results/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saad.LAKES\Desktop\Pavement-Temperature-Prediction\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C437E593-7E77-470E-BE0D-CA4DC6AF6157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BCBB2B-3B0B-464C-8887-770AA7667626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{63DD03F2-C25F-4FEC-9FD3-D8FFAFAFBABA}"/>
   </bookViews>
@@ -19,17 +19,21 @@
   </sheets>
   <definedNames>
     <definedName name="Slicer_Attention">#N/A</definedName>
+    <definedName name="Slicer_Dependent_Variable">#N/A</definedName>
     <definedName name="Slicer_Hours_Ahead">#N/A</definedName>
+    <definedName name="Slicer_Independent_Variables">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="14" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
         <x14:slicerCache r:id="rId5"/>
         <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
+        <x14:slicerCache r:id="rId8"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -52,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="25">
   <si>
     <t>Attention</t>
   </si>
@@ -113,12 +117,27 @@
   <si>
     <t>Seq2Seq</t>
   </si>
+  <si>
+    <t>Temperature, Solar, Pavement</t>
+  </si>
+  <si>
+    <t>Dependent Variable</t>
+  </si>
+  <si>
+    <t>Pavement</t>
+  </si>
+  <si>
+    <t>Independent Variables</t>
+  </si>
+  <si>
+    <t>Temperature,Pavement</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +146,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
@@ -140,10 +165,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -152,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -160,11 +196,50 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -944,19 +1019,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.0079818549785262</c:v>
+                  <c:v>3.1971332117897262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0101463709468685</c:v>
+                  <c:v>3.4647867384064832</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1514877080625645</c:v>
+                  <c:v>3.5290189176331239</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5426767587242587</c:v>
+                  <c:v>4.0704743505228356</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.6814087049809165</c:v>
+                  <c:v>4.4272601631441431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,19 +1155,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6.391382442590773</c:v>
+                  <c:v>3.8597555328309974</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3246772022361402</c:v>
+                  <c:v>3.4371642202869164</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.6903807124690626</c:v>
+                  <c:v>3.4970759608691941</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9135589438957474</c:v>
+                  <c:v>4.9879815728156824</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.3131987559032101</c:v>
+                  <c:v>3.6788693217829791</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2034,19 +2109,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>377253</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342901</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125775</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Hours Ahead">
@@ -2069,7 +2144,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2079,8 +2154,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5419725" y="38101"/>
-              <a:ext cx="5930328" cy="1181100"/>
+              <a:off x="9429751" y="66675"/>
+              <a:ext cx="3714750" cy="1011600"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2112,19 +2187,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>94951</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>135300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Attention">
@@ -2147,7 +2222,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2157,8 +2232,164 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="647699" y="57151"/>
-              <a:ext cx="4705351" cy="1180800"/>
+              <a:off x="5762625" y="76200"/>
+              <a:ext cx="3571875" cy="1011600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Independent Variables">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A849CA7B-2F7C-4F9D-BE9E-04AD2598E6B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Independent Variables"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="495300" y="76201"/>
+              <a:ext cx="3009900" cy="1009650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>135300</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Dependent Variable">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C370BF8-BE11-49FA-93B1-E51FAECC4441}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Dependent Variable"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3590924" y="76200"/>
+              <a:ext cx="2085975" cy="1011600"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2192,11 +2423,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="saad" refreshedDate="44158.387588541664" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{615D4E70-7A9E-45F9-8419-B7C4B78E1522}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="saad" refreshedDate="44158.698158796295" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="120" xr:uid="{615D4E70-7A9E-45F9-8419-B7C4B78E1522}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="9">
+  <cacheFields count="11">
     <cacheField name="Model" numFmtId="0">
       <sharedItems count="5">
         <s v="Wavenet"/>
@@ -2215,22 +2446,22 @@
       </sharedItems>
     </cacheField>
     <cacheField name="MAE" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.84001183762165499" maxValue="2.230857035990558"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.84001183762165499" maxValue="2.230857035990558"/>
     </cacheField>
     <cacheField name="MSE" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.3314802750536652" maxValue="8.9135589438957474"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.2119559901174757" maxValue="8.9135589438957474"/>
     </cacheField>
     <cacheField name="RMSE" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.1538978616210644" maxValue="2.9855583973347009"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.1538978616210644" maxValue="2.9855583973347009"/>
     </cacheField>
     <cacheField name="R2" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.84810035194260924" maxValue="0.97687885208408221"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.84810035194260924" maxValue="0.97687885208408221"/>
     </cacheField>
     <cacheField name="AGG" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.305074054358704E-2" maxValue="0.39618583422162418"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="2.305074054358704E-2" maxValue="0.39618583422162418"/>
     </cacheField>
     <cacheField name="Time Taken" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.66" maxValue="21.22"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="3.66" maxValue="21.22"/>
     </cacheField>
     <cacheField name="Hours Ahead" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6" count="6">
@@ -2240,6 +2471,17 @@
         <n v="4"/>
         <n v="5"/>
         <n v="6"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Independent Variables" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Temperature, Solar, Pavement"/>
+        <s v="Temperature,Pavement"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Dependent Variable" numFmtId="0">
+      <sharedItems count="1">
+        <s v="Pavement"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -2252,7 +2494,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="120">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -2263,6 +2505,8 @@
     <n v="9.2600331702575797E-2"/>
     <n v="6"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2274,6 +2518,8 @@
     <n v="9.6982008991396154E-2"/>
     <n v="6"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2285,6 +2531,8 @@
     <n v="9.8549009705031901E-2"/>
     <n v="6"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2296,6 +2544,8 @@
     <n v="0.11570640030242806"/>
     <n v="6"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2307,6 +2557,8 @@
     <n v="0.16104578175217787"/>
     <n v="6"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2318,6 +2570,8 @@
     <n v="0.25065490299547721"/>
     <n v="6"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2329,6 +2583,8 @@
     <n v="0.1254762371030603"/>
     <n v="6"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2340,6 +2596,8 @@
     <n v="0.14730764785781908"/>
     <n v="6"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2351,6 +2609,8 @@
     <n v="0.1653175542108288"/>
     <n v="6"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2362,6 +2622,8 @@
     <n v="0.19667850742530804"/>
     <n v="6"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2373,6 +2635,8 @@
     <n v="0.26870294854116555"/>
     <n v="6"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -2384,6 +2648,8 @@
     <n v="0.39618583422162418"/>
     <n v="6"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2395,6 +2661,8 @@
     <n v="2.4163966892245734E-2"/>
     <n v="5.32"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2406,6 +2674,8 @@
     <n v="4.9531994966810426E-2"/>
     <n v="5.32"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2417,6 +2687,8 @@
     <n v="7.9353300920432621E-2"/>
     <n v="5.32"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2428,6 +2700,8 @@
     <n v="0.11032915924798596"/>
     <n v="5.32"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2439,6 +2713,8 @@
     <n v="0.14358748101509741"/>
     <n v="5.32"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2450,6 +2726,8 @@
     <n v="0.22134571755863769"/>
     <n v="5.32"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2461,6 +2739,8 @@
     <n v="2.305074054358704E-2"/>
     <n v="5.4"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2472,6 +2752,8 @@
     <n v="4.8200595622177815E-2"/>
     <n v="5.4"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2483,6 +2765,8 @@
     <n v="6.1416718734832343E-2"/>
     <n v="5.4"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2494,6 +2778,8 @@
     <n v="9.442673980921823E-2"/>
     <n v="5.4"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2505,6 +2791,8 @@
     <n v="0.14635647604625238"/>
     <n v="5.4"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2516,6 +2804,8 @@
     <n v="0.24107230828449838"/>
     <n v="5.4"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2527,6 +2817,8 @@
     <n v="3.0126961181948572E-2"/>
     <n v="20.67"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2538,6 +2830,8 @@
     <n v="4.3631885078551889E-2"/>
     <n v="20.67"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2549,6 +2843,8 @@
     <n v="5.7093274967041883E-2"/>
     <n v="20.67"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2560,6 +2856,8 @@
     <n v="8.9335560513095255E-2"/>
     <n v="20.67"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2571,6 +2869,8 @@
     <n v="0.14696557025728288"/>
     <n v="20.67"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2582,6 +2882,8 @@
     <n v="0.22661694752851647"/>
     <n v="20.67"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2593,6 +2895,8 @@
     <n v="3.3619926665734434E-2"/>
     <n v="21.22"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2604,6 +2908,8 @@
     <n v="4.4880586702238712E-2"/>
     <n v="21.22"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2615,6 +2921,8 @@
     <n v="5.7220192709464913E-2"/>
     <n v="21.22"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2626,6 +2934,8 @@
     <n v="9.0982827589011148E-2"/>
     <n v="21.22"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2637,6 +2947,8 @@
     <n v="0.15607636715644996"/>
     <n v="21.22"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2648,6 +2960,8 @@
     <n v="0.25662990838455696"/>
     <n v="21.22"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2659,6 +2973,8 @@
     <n v="5.7137815057411771E-2"/>
     <n v="3.66"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2670,6 +2986,8 @@
     <n v="8.5398380120187203E-2"/>
     <n v="3.66"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2681,6 +2999,8 @@
     <n v="0.11019381648079042"/>
     <n v="3.66"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2692,6 +3012,8 @@
     <n v="0.1375692045063901"/>
     <n v="3.66"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2703,6 +3025,8 @@
     <n v="0.19241765292518614"/>
     <n v="3.66"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2714,6 +3038,8 @@
     <n v="0.32223356518128393"/>
     <n v="3.66"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2725,6 +3051,8 @@
     <n v="4.5263667364053788E-2"/>
     <n v="3.83"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2736,6 +3064,8 @@
     <n v="5.9763944559862579E-2"/>
     <n v="3.83"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2747,6 +3077,8 @@
     <n v="6.9252887370598065E-2"/>
     <n v="3.83"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2758,6 +3090,8 @@
     <n v="9.5371286970501776E-2"/>
     <n v="3.83"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2769,6 +3103,8 @@
     <n v="0.14589596969744775"/>
     <n v="3.83"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2780,6 +3116,8 @@
     <n v="0.23762732852613466"/>
     <n v="3.83"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2791,6 +3129,8 @@
     <n v="3.8683369862557479E-2"/>
     <n v="8.11"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2802,6 +3142,8 @@
     <n v="4.1951367127826412E-2"/>
     <n v="8.11"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2813,6 +3155,8 @@
     <n v="5.3778835137777731E-2"/>
     <n v="8.11"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2824,6 +3168,8 @@
     <n v="6.4024762796925372E-2"/>
     <n v="8.11"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2835,6 +3181,8 @@
     <n v="9.6459134625850526E-2"/>
     <n v="8.11"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2846,6 +3194,8 @@
     <n v="0.16871352804727779"/>
     <n v="8.11"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2857,6 +3207,8 @@
     <n v="5.6314286488135371E-2"/>
     <n v="8.16"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2868,6 +3220,8 @@
     <n v="5.961606258479242E-2"/>
     <n v="8.16"/>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2879,6 +3233,8 @@
     <n v="6.4812100514462026E-2"/>
     <n v="8.16"/>
     <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2890,6 +3246,8 @@
     <n v="8.8352845628347013E-2"/>
     <n v="8.16"/>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2901,6 +3259,8 @@
     <n v="0.14397095894939954"/>
     <n v="8.16"/>
     <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2912,14 +3272,796 @@
     <n v="0.24286342126365276"/>
     <n v="8.16"/>
     <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <m/>
+    <n v="1.65162025310385"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <m/>
+    <n v="2.8048411229416712"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <m/>
+    <n v="3.4425847454325584"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <m/>
+    <n v="4.7858100104510353"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <m/>
+    <n v="6.0358006100833732"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <m/>
+    <n v="7.5325753270782592"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.0094297892074424"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.4692592929266137"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <m/>
+    <n v="3.065043471535025"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <m/>
+    <n v="3.8356223360485862"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <m/>
+    <n v="4.8964111349927801"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <m/>
+    <n v="6.2025078573819838"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <n v="1.6306350215412018"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <n v="2.3001628934580478"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <n v="2.9543397537928522"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <n v="3.8353635600080875"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <n v="4.956391018059958"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <n v="6.5610404086404204"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <n v="1.58533275107712"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.1229215935092252"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.7922339465581136"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <n v="3.5684882916761125"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <n v="4.8061015655391923"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <n v="6.031831646131014"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <n v="1.3641341145637802"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <n v="1.8778766051562816"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <n v="2.9350723956185845"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <n v="3.8593643047964723"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <n v="4.7852192177328678"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <n v="5.8316305193120046"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <n v="1.2119559901174757"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.0312923803183289"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.9823886712161225"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <n v="3.8385196775699839"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <n v="4.8404706107016109"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <n v="6.021731217632003"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <m/>
+    <n v="1.2148814048269418"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <m/>
+    <n v="1.9628502539186456"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <m/>
+    <n v="2.9194772256516681"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <m/>
+    <n v="3.9247503625457711"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <m/>
+    <n v="4.9938734094713348"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <m/>
+    <n v="6.0525618432512118"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.8318906995687492"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.8210029611876877"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <m/>
+    <n v="3.1115299387349644"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <m/>
+    <n v="3.9289184867511469"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <m/>
+    <n v="5.2228375646384588"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <m/>
+    <n v="6.7100866564045658"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <n v="3.0510421622717896"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <n v="3.1102204527872637"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <n v="3.3593408940836254"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <n v="3.7011504171690541"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <n v="4.3997940912318301"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <n v="5.5206542048612635"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.147331769174035"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <n v="2.7612196249727181"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <n v="3.4989539055988814"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <n v="4.2800400334431643"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <n v="5.3768835349341524"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <n v="6.4852977642528886"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A33F6770-4ABB-4F87-976D-B13C6AD3E3D8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A33F6770-4ABB-4F87-976D-B13C6AD3E3D8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="9">
+  <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="6">
         <item x="3"/>
@@ -2959,12 +4101,25 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="7">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item h="1" x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
         <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="2">
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3103,11 +4258,11 @@
   <data>
     <tabular pivotCacheId="1413685035">
       <items count="6">
-        <i x="0"/>
-        <i x="1"/>
-        <i x="2"/>
-        <i x="3"/>
-        <i x="4"/>
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="2" s="1"/>
+        <i x="3" s="1"/>
+        <i x="4" s="1"/>
         <i x="5" s="1"/>
       </items>
     </tabular>
@@ -3138,26 +4293,61 @@
 </slicerCacheDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Independent_Variables" xr10:uid="{41036976-980B-4642-AD9A-EDE115F30783}" sourceName="Independent Variables">
+  <pivotTables>
+    <pivotTable tabId="2" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1413685035">
+      <items count="2">
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Dependent_Variable" xr10:uid="{CFAEF613-4F77-41A3-A0B2-1F7AA382D04C}" sourceName="Dependent Variable">
+  <pivotTables>
+    <pivotTable tabId="2" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1413685035">
+      <items count="1">
+        <i x="0" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
   <slicer name="Hours Ahead" xr10:uid="{64F0BDE9-715E-4C50-8396-37376C2EED05}" cache="Slicer_Hours_Ahead" caption="Hours Ahead" columnCount="6" rowHeight="432000"/>
-  <slicer name="Attention" xr10:uid="{5D8ED07C-F289-44ED-A447-4A4EF47F8E5C}" cache="Slicer_Attention" caption="Attention" columnCount="2" style="SlicerStyleLight2" rowHeight="576000"/>
+  <slicer name="Attention" xr10:uid="{5D8ED07C-F289-44ED-A447-4A4EF47F8E5C}" cache="Slicer_Attention" caption="Attention" columnCount="2" style="SlicerStyleLight2" rowHeight="468000"/>
+  <slicer name="Independent Variables" xr10:uid="{BF468159-37B0-4AC9-82DA-4D81AFD31B96}" cache="Slicer_Independent_Variables" caption="Independent Variables" rowHeight="241300"/>
+  <slicer name="Dependent Variable" xr10:uid="{91F5BB25-3613-4985-AFFC-08E58075BB73}" cache="Slicer_Dependent_Variable" caption="Dependent Variable" style="SlicerStyleOther1" rowHeight="471600"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A40C5364-D532-4850-BD71-B2C37FA582EC}" name="Table1" displayName="Table1" ref="A1:I61" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:I61" xr:uid="{ED0D47FB-18B8-4C67-9670-3E2CBE517802}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A40C5364-D532-4850-BD71-B2C37FA582EC}" name="Table1" displayName="Table1" ref="A1:K121" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:K121" xr:uid="{ED0D47FB-18B8-4C67-9670-3E2CBE517802}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{CF545063-03CF-401E-930A-816F89247E2E}" name="Model"/>
-    <tableColumn id="2" xr3:uid="{D95F79F9-E1DE-4634-A376-76E193012D40}" name="Attention" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{FB734E54-1D25-4C2D-AD8B-39527EEDAABA}" name="MAE" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{60154C47-3BE3-4E5B-A931-1E999CC0C5FE}" name="MSE" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{9E5FEA15-4FB9-43EA-B2D3-21FF74A30FAA}" name="RMSE" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{8F099E94-3629-4105-8223-CA7DDF8D9C37}" name="R2" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{D27EA600-3E43-4725-ABC3-B81E508957A2}" name="AGG" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{1D05D863-E2CE-4563-BB89-51FB596E89D4}" name="Time Taken" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{DC3A857A-91A6-4BE6-8A96-AB493AD8E254}" name="Hours Ahead" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{D95F79F9-E1DE-4634-A376-76E193012D40}" name="Attention" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{FB734E54-1D25-4C2D-AD8B-39527EEDAABA}" name="MAE" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{60154C47-3BE3-4E5B-A931-1E999CC0C5FE}" name="MSE" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{9E5FEA15-4FB9-43EA-B2D3-21FF74A30FAA}" name="RMSE" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{8F099E94-3629-4105-8223-CA7DDF8D9C37}" name="R2" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{D27EA600-3E43-4725-ABC3-B81E508957A2}" name="AGG" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{1D05D863-E2CE-4563-BB89-51FB596E89D4}" name="Time Taken" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{DC3A857A-91A6-4BE6-8A96-AB493AD8E254}" name="Hours Ahead" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{731B20BD-426E-4FB0-B4D6-021D14A2B4BD}" name="Independent Variables" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{5E360D0B-618E-4414-BD1C-63CE4A717476}" name="Dependent Variable" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3501,13 +4691,13 @@
         <v>19</v>
       </c>
       <c r="B5" s="4">
-        <v>5.0079818549785262</v>
+        <v>3.1971332117897262</v>
       </c>
       <c r="C5" s="4">
-        <v>6.391382442590773</v>
+        <v>3.8597555328309974</v>
       </c>
       <c r="D5" s="4">
-        <v>5.6996821487846496</v>
+        <v>3.528444372310362</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3515,13 +4705,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="4">
-        <v>6.0101463709468685</v>
+        <v>3.4647867384064832</v>
       </c>
       <c r="C6" s="4">
-        <v>6.3246772022361402</v>
+        <v>3.4371642202869164</v>
       </c>
       <c r="D6" s="4">
-        <v>6.1674117865915044</v>
+        <v>3.4509754793467007</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3529,13 +4719,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="4">
-        <v>6.1514877080625645</v>
+        <v>3.5290189176331239</v>
       </c>
       <c r="C7" s="4">
-        <v>6.6903807124690626</v>
+        <v>3.4970759608691941</v>
       </c>
       <c r="D7" s="4">
-        <v>6.4209342102658136</v>
+        <v>3.5130474392511597</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3543,13 +4733,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="4">
-        <v>6.5426767587242587</v>
+        <v>4.0704743505228356</v>
       </c>
       <c r="C8" s="4">
-        <v>8.9135589438957474</v>
+        <v>4.9879815728156824</v>
       </c>
       <c r="D8" s="4">
-        <v>7.7281178513100031</v>
+        <v>4.5292279616692595</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3557,13 +4747,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="4">
-        <v>7.6814087049809165</v>
+        <v>4.4272601631441431</v>
       </c>
       <c r="C9" s="4">
-        <v>6.3131987559032101</v>
+        <v>3.6788693217829791</v>
       </c>
       <c r="D9" s="4">
-        <v>6.9973037304420629</v>
+        <v>4.0530647424635609</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3571,13 +4761,13 @@
         <v>14</v>
       </c>
       <c r="B10" s="4">
-        <v>6.2787402795386269</v>
+        <v>3.7377346762992638</v>
       </c>
       <c r="C10" s="4">
-        <v>6.9266396114189863</v>
+        <v>3.8921693217171542</v>
       </c>
       <c r="D10" s="4">
-        <v>6.6026899454788062</v>
+        <v>3.8149519990082088</v>
       </c>
     </row>
   </sheetData>
@@ -3590,7 +4780,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3609,20 +4799,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380DC729-2475-4475-80B1-F9475DF84150}">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -3650,8 +4843,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3679,8 +4878,14 @@
       <c r="I2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3708,8 +4913,14 @@
       <c r="I3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3737,8 +4948,14 @@
       <c r="I4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3766,8 +4983,14 @@
       <c r="I5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3795,8 +5018,14 @@
       <c r="I6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3824,8 +5053,14 @@
       <c r="I7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3853,8 +5088,14 @@
       <c r="I8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3882,8 +5123,14 @@
       <c r="I9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3911,8 +5158,14 @@
       <c r="I10" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3940,8 +5193,14 @@
       <c r="I11" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3969,8 +5228,14 @@
       <c r="I12" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -3998,8 +5263,14 @@
       <c r="I13" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -4027,8 +5298,14 @@
       <c r="I14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -4056,8 +5333,14 @@
       <c r="I15" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4085,8 +5368,14 @@
       <c r="I16" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -4114,8 +5403,14 @@
       <c r="I17" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -4143,8 +5438,14 @@
       <c r="I18" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -4172,8 +5473,14 @@
       <c r="I19" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -4201,8 +5508,14 @@
       <c r="I20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -4230,8 +5543,14 @@
       <c r="I21" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -4259,8 +5578,14 @@
       <c r="I22" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -4288,8 +5613,14 @@
       <c r="I23" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -4317,8 +5648,14 @@
       <c r="I24" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -4346,8 +5683,14 @@
       <c r="I25" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -4375,8 +5718,14 @@
       <c r="I26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -4404,8 +5753,14 @@
       <c r="I27" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -4433,8 +5788,14 @@
       <c r="I28" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -4462,8 +5823,14 @@
       <c r="I29" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -4491,8 +5858,14 @@
       <c r="I30" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -4520,8 +5893,14 @@
       <c r="I31" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -4549,8 +5928,14 @@
       <c r="I32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -4578,8 +5963,14 @@
       <c r="I33" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -4607,8 +5998,14 @@
       <c r="I34" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -4636,8 +6033,14 @@
       <c r="I35" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -4665,8 +6068,14 @@
       <c r="I36" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -4694,8 +6103,14 @@
       <c r="I37" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -4723,8 +6138,14 @@
       <c r="I38" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -4752,8 +6173,14 @@
       <c r="I39" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -4781,8 +6208,14 @@
       <c r="I40" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -4810,8 +6243,14 @@
       <c r="I41" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -4839,8 +6278,14 @@
       <c r="I42" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -4868,8 +6313,14 @@
       <c r="I43" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -4897,8 +6348,14 @@
       <c r="I44" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -4926,8 +6383,14 @@
       <c r="I45" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -4955,8 +6418,14 @@
       <c r="I46" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -4984,8 +6453,14 @@
       <c r="I47" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -5013,8 +6488,14 @@
       <c r="I48" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -5042,8 +6523,14 @@
       <c r="I49" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -5071,8 +6558,14 @@
       <c r="I50" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -5100,8 +6593,14 @@
       <c r="I51" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -5129,8 +6628,14 @@
       <c r="I52" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -5158,8 +6663,14 @@
       <c r="I53" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -5187,8 +6698,14 @@
       <c r="I54" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -5216,8 +6733,14 @@
       <c r="I55" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -5245,8 +6768,14 @@
       <c r="I56" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -5274,8 +6803,14 @@
       <c r="I57" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -5303,8 +6838,14 @@
       <c r="I58" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -5332,8 +6873,14 @@
       <c r="I59" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -5361,8 +6908,14 @@
       <c r="I60" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -5389,6 +6942,1512 @@
       </c>
       <c r="I61" s="1">
         <v>6</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1">
+        <v>1.65162025310385</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1">
+        <v>1</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1">
+        <v>2.8048411229416712</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1">
+        <v>2</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1">
+        <v>3.4425847454325584</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1">
+        <v>3</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1">
+        <v>4.7858100104510353</v>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1">
+        <v>4</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1">
+        <v>6.0358006100833732</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1">
+        <v>5</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1">
+        <v>7.5325753270782592</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1">
+        <v>6</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1">
+        <v>2.0094297892074424</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1">
+        <v>1</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1">
+        <v>2.4692592929266137</v>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1">
+        <v>2</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1">
+        <v>3.065043471535025</v>
+      </c>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1">
+        <v>3</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1">
+        <v>3.8356223360485862</v>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1">
+        <v>4</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1">
+        <v>4.8964111349927801</v>
+      </c>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1">
+        <v>5</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1">
+        <v>6.2025078573819838</v>
+      </c>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1">
+        <v>6</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1">
+        <v>1.6306350215412018</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1">
+        <v>1</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1">
+        <v>2.3001628934580478</v>
+      </c>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1">
+        <v>2</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1">
+        <v>2.9543397537928522</v>
+      </c>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1">
+        <v>3</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1">
+        <v>3.8353635600080875</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1">
+        <v>4</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1">
+        <v>4.956391018059958</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1">
+        <v>5</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1">
+        <v>6.5610404086404204</v>
+      </c>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1">
+        <v>6</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1">
+        <v>1.58533275107712</v>
+      </c>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1">
+        <v>1</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1">
+        <v>2.1229215935092252</v>
+      </c>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1">
+        <v>2</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1">
+        <v>2.7922339465581136</v>
+      </c>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1">
+        <v>3</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1">
+        <v>3.5684882916761125</v>
+      </c>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1">
+        <v>4</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1">
+        <v>4.8061015655391923</v>
+      </c>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1">
+        <v>5</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1">
+        <v>6.031831646131014</v>
+      </c>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1">
+        <v>6</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1">
+        <v>1.3641341145637802</v>
+      </c>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1">
+        <v>1</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1">
+        <v>1.8778766051562816</v>
+      </c>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1">
+        <v>2</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1">
+        <v>2.9350723956185845</v>
+      </c>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1">
+        <v>3</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1">
+        <v>3.8593643047964723</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1">
+        <v>4</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1">
+        <v>4.7852192177328678</v>
+      </c>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1">
+        <v>5</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1">
+        <v>5.8316305193120046</v>
+      </c>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1">
+        <v>6</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1">
+        <v>1.2119559901174757</v>
+      </c>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1">
+        <v>1</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1">
+        <v>2.0312923803183289</v>
+      </c>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1">
+        <v>2</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1">
+        <v>2.9823886712161225</v>
+      </c>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1">
+        <v>3</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1">
+        <v>3.8385196775699839</v>
+      </c>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1">
+        <v>4</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1">
+        <v>4.8404706107016109</v>
+      </c>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1">
+        <v>5</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1">
+        <v>6.021731217632003</v>
+      </c>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1">
+        <v>6</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>19</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1">
+        <v>1.2148814048269418</v>
+      </c>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1">
+        <v>1</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>19</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1">
+        <v>1.9628502539186456</v>
+      </c>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1">
+        <v>2</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>19</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1">
+        <v>2.9194772256516681</v>
+      </c>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1">
+        <v>3</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>19</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1">
+        <v>3.9247503625457711</v>
+      </c>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1">
+        <v>4</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>19</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1">
+        <v>4.9938734094713348</v>
+      </c>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1">
+        <v>5</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1">
+        <v>6.0525618432512118</v>
+      </c>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1">
+        <v>6</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>19</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1">
+        <v>2.8318906995687492</v>
+      </c>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1">
+        <v>1</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>19</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1">
+        <v>2.8210029611876877</v>
+      </c>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1">
+        <v>2</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>19</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1">
+        <v>3.1115299387349644</v>
+      </c>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1">
+        <v>3</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>19</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1">
+        <v>3.9289184867511469</v>
+      </c>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1">
+        <v>4</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>19</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1">
+        <v>5.2228375646384588</v>
+      </c>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1">
+        <v>5</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>19</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1">
+        <v>6.7100866564045658</v>
+      </c>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1">
+        <v>6</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1">
+        <v>3.0510421622717896</v>
+      </c>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1">
+        <v>1</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1">
+        <v>3.1102204527872637</v>
+      </c>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1">
+        <v>2</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1">
+        <v>3.3593408940836254</v>
+      </c>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1">
+        <v>3</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>9</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1">
+        <v>3.7011504171690541</v>
+      </c>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1">
+        <v>4</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1">
+        <v>4.3997940912318301</v>
+      </c>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1">
+        <v>5</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1">
+        <v>5.5206542048612635</v>
+      </c>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1">
+        <v>6</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>9</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1">
+        <v>2.147331769174035</v>
+      </c>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1">
+        <v>1</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>9</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1">
+        <v>2.7612196249727181</v>
+      </c>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1">
+        <v>2</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>9</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1">
+        <v>3.4989539055988814</v>
+      </c>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1">
+        <v>3</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1">
+        <v>4.2800400334431643</v>
+      </c>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1">
+        <v>4</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1">
+        <v>5.3768835349341524</v>
+      </c>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1">
+        <v>5</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>9</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1">
+        <v>6.4852977642528886</v>
+      </c>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1">
+        <v>6</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the screenshot of the dashboard and initalized the file
</commit_message>
<xml_diff>
--- a/Results/Dashboard.xlsx
+++ b/Results/Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saad.LAKES\Desktop\Pavement-Temperature-Prediction\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381D121B-53E8-46A1-B792-E78F6E9B07AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81426377-90C0-4B34-845A-E57CD5A02633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63DD03F2-C25F-4FEC-9FD3-D8FFAFAFBABA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{63DD03F2-C25F-4FEC-9FD3-D8FFAFAFBABA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -911,19 +911,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Wavenet</c:v>
+                  <c:v>Seq2Seq</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>LSTM</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Seq2Seq</c:v>
+                  <c:v>ConvLSTM</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ConvLSTM</c:v>
+                  <c:v>CNN-LSTM</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CNN-LSTM</c:v>
+                  <c:v>Wavenet</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -935,19 +935,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.5206542048612635</c:v>
+                  <c:v>4.5261623352283991</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8316305193120046</c:v>
+                  <c:v>4.8919237217338338</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0525618432512118</c:v>
+                  <c:v>4.9063290317872106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5610404086404204</c:v>
+                  <c:v>5.0426266225501202</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.5325753270782592</c:v>
+                  <c:v>5.287356284352799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1047,19 +1047,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Wavenet</c:v>
+                  <c:v>Seq2Seq</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>LSTM</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Seq2Seq</c:v>
+                  <c:v>ConvLSTM</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ConvLSTM</c:v>
+                  <c:v>CNN-LSTM</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CNN-LSTM</c:v>
+                  <c:v>Wavenet</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1071,19 +1071,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6.4852977642528886</c:v>
+                  <c:v>5.4884722397578569</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.021731217632003</c:v>
+                  <c:v>4.7177383560485842</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7100866564045658</c:v>
+                  <c:v>4.7815969212582674</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.031831646131014</c:v>
+                  <c:v>4.6577333375320142</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2025078573819838</c:v>
+                  <c:v>5.5822341342530812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3687,7 +3687,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A33F6770-4ABB-4F87-976D-B13C6AD3E3D8}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A33F6770-4ABB-4F87-976D-B13C6AD3E3D8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -3725,25 +3725,25 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0">
       <items count="7">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item h="1" x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
         <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" x="1"/>
+        <item x="1"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" m="1" x="1"/>
+        <item m="1" x="1"/>
         <item x="0"/>
         <item t="default"/>
       </items>
@@ -3760,19 +3760,19 @@
   </rowFields>
   <rowItems count="6">
     <i>
-      <x v="3"/>
+      <x v="4"/>
     </i>
     <i>
       <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
     </i>
     <i>
       <x v="1"/>
     </i>
     <i>
       <x/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
@@ -3889,11 +3889,11 @@
   <data>
     <tabular pivotCacheId="1413685035">
       <items count="6">
-        <i x="0"/>
-        <i x="1"/>
-        <i x="2"/>
-        <i x="3"/>
-        <i x="4"/>
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="2" s="1"/>
+        <i x="3" s="1"/>
+        <i x="4" s="1"/>
         <i x="5" s="1"/>
       </items>
     </tabular>
@@ -3933,7 +3933,7 @@
     <tabular pivotCacheId="1413685035">
       <items count="2">
         <i x="0" s="1"/>
-        <i x="1" nd="1"/>
+        <i x="1" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -3963,7 +3963,7 @@
   <data>
     <tabular pivotCacheId="1413685035">
       <items count="2">
-        <i x="1"/>
+        <i x="1" s="1"/>
         <i x="0" s="1"/>
       </items>
     </tabular>
@@ -3990,9 +3990,9 @@
     <tableColumn id="3" xr3:uid="{FB734E54-1D25-4C2D-AD8B-39527EEDAABA}" name="MAE" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{60154C47-3BE3-4E5B-A931-1E999CC0C5FE}" name="MSE" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{DC3A857A-91A6-4BE6-8A96-AB493AD8E254}" name="Hours Ahead" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{C20A1A75-C133-4164-BAFF-BCC40FE1F532}" name="Lag" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{731B20BD-426E-4FB0-B4D6-021D14A2B4BD}" name="Independent Variables" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{5E360D0B-618E-4414-BD1C-63CE4A717476}" name="Dependent Variable" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{C20A1A75-C133-4164-BAFF-BCC40FE1F532}" name="Lag" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{731B20BD-426E-4FB0-B4D6-021D14A2B4BD}" name="Independent Variables" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{5E360D0B-618E-4414-BD1C-63CE4A717476}" name="Dependent Variable" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4297,8 +4297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380DC729-2475-4475-80B1-F9475DF84150}">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7264,16 +7264,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4">
-        <v>5.5206542048612635</v>
+        <v>4.5261623352283991</v>
       </c>
       <c r="C5" s="4">
-        <v>6.4852977642528886</v>
+        <v>5.4884722397578569</v>
       </c>
       <c r="D5" s="4">
-        <v>6.002975984557076</v>
+        <v>5.0073172874931275</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -7281,55 +7281,55 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>5.8316305193120046</v>
+        <v>4.8919237217338338</v>
       </c>
       <c r="C6" s="4">
-        <v>6.021731217632003</v>
+        <v>4.7177383560485842</v>
       </c>
       <c r="D6" s="4">
-        <v>5.9266808684720038</v>
+        <v>4.8048310388912086</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>6.0525618432512118</v>
+        <v>4.9063290317872106</v>
       </c>
       <c r="C7" s="4">
-        <v>6.7100866564045658</v>
+        <v>4.7815969212582674</v>
       </c>
       <c r="D7" s="4">
-        <v>6.3813242498278893</v>
+        <v>4.8439629765227394</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4">
-        <v>6.5610404086404204</v>
+        <v>5.0426266225501202</v>
       </c>
       <c r="C8" s="4">
-        <v>6.031831646131014</v>
+        <v>4.6577333375320142</v>
       </c>
       <c r="D8" s="4">
-        <v>6.2964360273857167</v>
+        <v>4.8501799800410659</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4">
-        <v>7.5325753270782592</v>
+        <v>5.287356284352799</v>
       </c>
       <c r="C9" s="4">
-        <v>6.2025078573819838</v>
+        <v>5.5822341342530812</v>
       </c>
       <c r="D9" s="4">
-        <v>6.8675415922301219</v>
+        <v>5.4347952093029406</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7337,13 +7337,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>6.2996924606286315</v>
+        <v>4.9308795991304741</v>
       </c>
       <c r="C10" s="4">
-        <v>6.2902910283604907</v>
+        <v>5.0455549977699601</v>
       </c>
       <c r="D10" s="4">
-        <v>6.2949917444945616</v>
+        <v>4.9882172984502153</v>
       </c>
     </row>
   </sheetData>
@@ -7355,8 +7355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39C62B1-CAD0-433A-99ED-C9AC0DBA5B64}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB19" sqref="AB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>